<commit_message>
Mise à jour tableau de synthèse E5
</commit_message>
<xml_diff>
--- a/public/e5/annexe8-1_tableau_synthese.xlsx
+++ b/public/e5/annexe8-1_tableau_synthese.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frani\OneDrive\Bureau\project\public\e5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1691B9B-0F2C-429A-8E1A-412DFC5F93B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0CD2381-F033-4CA2-B90C-9CCDBB7982EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -86,9 +86,6 @@
 ▸Développer son projet professionnel</t>
   </si>
   <si>
-    <t>Centre de formation :</t>
-  </si>
-  <si>
     <t>▢ SISR</t>
   </si>
   <si>
@@ -135,6 +132,30 @@
   </si>
   <si>
     <t>Mission 3 : Mise en Place d'une Solution pour l'Administration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elaboration d'une veille technologique sur la 6G</t>
+  </si>
+  <si>
+    <t>Assistance aux utilisateurs</t>
+  </si>
+  <si>
+    <t>Recensement matériel informatique</t>
+  </si>
+  <si>
+    <t>Déploiement et configuration des postes de travail</t>
+  </si>
+  <si>
+    <t>Installation de matériel informatique : matériel de bureau, matériel de réunion en visoconférence</t>
+  </si>
+  <si>
+    <t>Savoir se procurer les procédures nécessaires à la résolution d'un problème</t>
+  </si>
+  <si>
+    <t>Résolution de problèmes logiciels</t>
+  </si>
+  <si>
+    <t>Centre de formation : IRIS</t>
   </si>
 </sst>
 </file>
@@ -208,12 +229,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF242424"/>
-      <name val="Segoe UI"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF242424"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -623,7 +644,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -688,15 +709,45 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -730,37 +781,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1176,13 +1205,13 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="70.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="77.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
     <col min="3" max="8" width="18.7109375" style="1" customWidth="1"/>
     <col min="9" max="43" width="11.42578125" customWidth="1"/>
@@ -1199,7 +1228,7 @@
       <c r="E1" s="24"/>
       <c r="F1" s="24"/>
       <c r="G1" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="24"/>
     </row>
@@ -1216,58 +1245,58 @@
       <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="43"/>
+      <c r="A3" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="26"/>
+      <c r="H3" s="32"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="A4" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="21" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="A5" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>21</v>
+      <c r="A6" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>0</v>
@@ -1289,8 +1318,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1346,16 +1375,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="A8" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1393,8 +1422,8 @@
       <c r="AQ8"/>
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="46" t="s">
-        <v>27</v>
+      <c r="A9" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="16"/>
@@ -1402,7 +1431,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="44"/>
+      <c r="H9" s="22"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1439,9 +1468,9 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
-        <v>28</v>
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="46" t="s">
+        <v>30</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="17"/>
@@ -1449,7 +1478,7 @@
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
+      <c r="H10" s="22"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1486,9 +1515,9 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
-        <v>29</v>
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="47" t="s">
+        <v>27</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="17"/>
@@ -1533,9 +1562,9 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="45" t="s">
-        <v>30</v>
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="47" t="s">
+        <v>28</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="17"/>
@@ -1581,7 +1610,9 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
+      <c r="A13" s="47" t="s">
+        <v>29</v>
+      </c>
       <c r="B13" s="10"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -1626,7 +1657,7 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="10"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -1851,16 +1882,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
+      <c r="A19" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="40"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1898,11 +1929,13 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
+      <c r="A20" s="47" t="s">
+        <v>31</v>
+      </c>
       <c r="B20" s="10"/>
       <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="18"/>
@@ -1943,9 +1976,11 @@
       <c r="AQ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
+      <c r="A21" s="50" t="s">
+        <v>32</v>
+      </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="17"/>
+      <c r="C21" s="48"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
@@ -1988,13 +2023,15 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
+      <c r="A22" s="50" t="s">
+        <v>33</v>
+      </c>
       <c r="B22" s="10"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
+      <c r="G22" s="48"/>
       <c r="H22" s="18"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -2213,16 +2250,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
+      <c r="A27" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="40"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2260,13 +2297,15 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
+      <c r="A28" s="49" t="s">
+        <v>34</v>
+      </c>
       <c r="B28" s="10"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
+      <c r="G28" s="48"/>
       <c r="H28" s="18"/>
       <c r="I28"/>
       <c r="J28"/>
@@ -2305,7 +2344,9 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
+      <c r="A29" s="49" t="s">
+        <v>35</v>
+      </c>
       <c r="B29" s="10"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -2350,13 +2391,15 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
+      <c r="A30" s="49" t="s">
+        <v>36</v>
+      </c>
       <c r="B30" s="10"/>
       <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
+      <c r="G30" s="48"/>
       <c r="H30" s="18"/>
       <c r="I30"/>
       <c r="J30"/>
@@ -2667,11 +2710,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2679,6 +2717,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Ajout aperçu PDF du tableau de synthèse E5
</commit_message>
<xml_diff>
--- a/public/e5/annexe8-1_tableau_synthese.xlsx
+++ b/public/e5/annexe8-1_tableau_synthese.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frani\OneDrive\Bureau\project\public\e5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4076EB01-9217-47B0-B93B-CC73EDC9E5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D7AAE6-CBE8-4454-8DF2-EE60E7981FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,7 +165,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -229,12 +229,26 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF242424"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -253,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -265,21 +279,6 @@
       <left style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
       <right/>
       <top style="thin">
         <color theme="2" tint="-0.749992370372631"/>
@@ -314,7 +313,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </left>
       <right style="thin">
@@ -332,73 +331,13 @@
       <left style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color theme="2" tint="-0.749992370372631"/>
       </right>
       <top style="medium">
         <color theme="2" tint="-0.749992370372631"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
         <color theme="2" tint="-0.749992370372631"/>
       </bottom>
       <diagonal/>
@@ -455,36 +394,6 @@
         <color theme="2" tint="-0.749992370372631"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -639,12 +548,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -661,135 +611,114 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1205,8 +1134,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1219,83 +1148,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="31" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="32"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="28"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="14" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="45"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1318,8 +1247,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1375,16 +1304,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1422,16 +1351,16 @@
       <c r="AQ8"/>
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="22"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="36"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1469,16 +1398,16 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="36"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1516,16 +1445,16 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1563,16 +1492,16 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1610,16 +1539,16 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="18"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1657,14 +1586,14 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="47"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="18"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1702,14 +1631,14 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1747,14 +1676,14 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1792,14 +1721,14 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="18"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1837,14 +1766,14 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="18"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1885,13 +1814,13 @@
       <c r="A19" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1929,16 +1858,16 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="18"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1976,16 +1905,16 @@
       <c r="AQ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="18"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -2023,16 +1952,16 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="18"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="35"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2070,14 +1999,14 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="18"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2115,14 +2044,14 @@
       <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="18"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2160,14 +2089,14 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="18"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2205,14 +2134,14 @@
       <c r="AQ25"/>
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="18"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2253,13 +2182,13 @@
       <c r="A27" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="40"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2297,16 +2226,16 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="18"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="35"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2344,16 +2273,16 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="18"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2391,16 +2320,16 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="18"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="35"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2438,14 +2367,14 @@
       <c r="AQ30"/>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="18"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2483,14 +2412,14 @@
       <c r="AQ31"/>
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="11"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="18"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2528,14 +2457,14 @@
       <c r="AQ32"/>
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="11"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="18"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2572,15 +2501,15 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="20"/>
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="37"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2710,6 +2639,11 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2717,11 +2651,6 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
E5 final : missions, alternance, onboarding et tableau de synthèse
</commit_message>
<xml_diff>
--- a/public/e5/annexe8-1_tableau_synthese.xlsx
+++ b/public/e5/annexe8-1_tableau_synthese.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frani\OneDrive\Bureau\project\public\e5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D7AAE6-CBE8-4454-8DF2-EE60E7981FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63785DCB-8034-432C-A602-4C503653E9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -594,7 +594,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -632,64 +632,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -704,9 +647,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -718,6 +658,69 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1134,70 +1137,70 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="77.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
     <col min="3" max="8" width="18.7109375" style="1" customWidth="1"/>
     <col min="9" max="43" width="11.42578125" customWidth="1"/>
     <col min="44" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="15"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="27" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="28"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="32"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
@@ -1209,22 +1212,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="20"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="39" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1247,8 +1250,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1304,16 +1307,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1351,16 +1354,18 @@
       <c r="AQ8"/>
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="36"/>
+      <c r="B9" s="44">
+        <v>45689</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1398,16 +1403,18 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="36"/>
+      <c r="B10" s="44">
+        <v>45717</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1445,16 +1452,18 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
+      <c r="B11" s="44">
+        <v>45913</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="16"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1492,16 +1501,18 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
+      <c r="B12" s="44">
+        <v>45950</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="16"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1539,16 +1550,18 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
+      <c r="B13" s="44">
+        <v>45988</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="16"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1586,14 +1599,14 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="30"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1631,14 +1644,13 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="37"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
+      <c r="A15" s="18"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1676,14 +1688,14 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="37"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1721,14 +1733,14 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="37"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1766,14 +1778,14 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1858,16 +1870,18 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
+      <c r="B20" s="44">
+        <v>45689</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1905,16 +1919,18 @@
       <c r="AQ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
+      <c r="B21" s="44">
+        <v>45689</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -1952,16 +1968,18 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="35"/>
+      <c r="B22" s="44">
+        <v>45689</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="16"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -1999,14 +2017,14 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="43"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2044,14 +2062,14 @@
       <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="43"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2089,14 +2107,14 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="43"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2134,14 +2152,14 @@
       <c r="AQ25"/>
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="43"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2226,16 +2244,18 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="35"/>
+      <c r="B28" s="44">
+        <v>45536</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="16"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2273,16 +2293,18 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
+      <c r="B29" s="44">
+        <v>45536</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2320,16 +2342,18 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="35"/>
+      <c r="B30" s="44">
+        <v>45536</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="16"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2367,14 +2391,14 @@
       <c r="AQ30"/>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="37"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2412,14 +2436,14 @@
       <c r="AQ31"/>
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="37"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2457,14 +2481,14 @@
       <c r="AQ32"/>
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="37"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="35"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2502,14 +2526,14 @@
       <c r="AQ33"/>
     </row>
     <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="37"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2639,11 +2663,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2651,6 +2670,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Mise à jour Tableau
</commit_message>
<xml_diff>
--- a/public/e5/annexe8-1_tableau_synthese.xlsx
+++ b/public/e5/annexe8-1_tableau_synthese.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frani\OneDrive\Bureau\project\public\e5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63785DCB-8034-432C-A602-4C503653E9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1C8E19-1D97-4A27-B07C-D1766B65E1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -156,6 +156,24 @@
   </si>
   <si>
     <t>Adresse URL du portfolio : https://tino-franic-portfolio.netlify.app/</t>
+  </si>
+  <si>
+    <t>Rédaction de procédure de onboarding IT</t>
+  </si>
+  <si>
+    <t>Installation et paramétrage d’une application avec licence serveur (MAROS)</t>
+  </si>
+  <si>
+    <t>Création de canaux Microsoft Teams pour des utilisateurs</t>
+  </si>
+  <si>
+    <t>Formation à l’utilisation du paperboard Samsung (pour plusieurs personnes)</t>
+  </si>
+  <si>
+    <t>Gestion des accès SharePoint / bases de données</t>
+  </si>
+  <si>
+    <t>Gestion des commandes de téléphones et forfaits</t>
   </si>
 </sst>
 </file>
@@ -165,7 +183,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -252,6 +270,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -594,7 +617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -659,9 +682,45 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -686,41 +745,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1137,8 +1173,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1151,56 +1187,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="31" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="32"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="44"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
@@ -1212,22 +1248,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="32" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1250,15 +1286,15 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="49" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -1307,16 +1343,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1357,7 +1393,7 @@
       <c r="A9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="24">
         <v>45689</v>
       </c>
       <c r="C9" s="15"/>
@@ -1406,7 +1442,7 @@
       <c r="A10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="24">
         <v>45717</v>
       </c>
       <c r="C10" s="16"/>
@@ -1455,7 +1491,7 @@
       <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="44">
+      <c r="B11" s="24">
         <v>45913</v>
       </c>
       <c r="C11" s="17"/>
@@ -1504,7 +1540,7 @@
       <c r="A12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="44">
+      <c r="B12" s="24">
         <v>45950</v>
       </c>
       <c r="C12" s="17"/>
@@ -1553,7 +1589,7 @@
       <c r="A13" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="44">
+      <c r="B13" s="24">
         <v>45988</v>
       </c>
       <c r="C13" s="17"/>
@@ -1823,16 +1859,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1873,7 +1909,7 @@
       <c r="A20" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="44">
+      <c r="B20" s="24">
         <v>45689</v>
       </c>
       <c r="C20" s="16"/>
@@ -1922,7 +1958,7 @@
       <c r="A21" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="44">
+      <c r="B21" s="24">
         <v>45689</v>
       </c>
       <c r="C21" s="17"/>
@@ -1971,7 +2007,7 @@
       <c r="A22" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="44">
+      <c r="B22" s="24">
         <v>45689</v>
       </c>
       <c r="C22" s="16"/>
@@ -2017,13 +2053,17 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="23"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="45">
+        <v>45778</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
       <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
       <c r="H23" s="16"/>
       <c r="I23"/>
       <c r="J23"/>
@@ -2062,13 +2102,15 @@
       <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="23"/>
+      <c r="A24" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="B24" s="14"/>
-      <c r="C24" s="16"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
+      <c r="E24" s="17"/>
       <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
+      <c r="G24" s="17"/>
       <c r="H24" s="16"/>
       <c r="I24"/>
       <c r="J24"/>
@@ -2107,13 +2149,15 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
+      <c r="A25" s="48" t="s">
+        <v>42</v>
+      </c>
       <c r="B25" s="14"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
+      <c r="G25" s="17"/>
       <c r="H25" s="16"/>
       <c r="I25"/>
       <c r="J25"/>
@@ -2197,16 +2241,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2247,7 +2291,7 @@
       <c r="A28" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="44">
+      <c r="B28" s="24">
         <v>45536</v>
       </c>
       <c r="C28" s="17"/>
@@ -2296,7 +2340,7 @@
       <c r="A29" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="44">
+      <c r="B29" s="24">
         <v>45536</v>
       </c>
       <c r="C29" s="16"/>
@@ -2345,7 +2389,7 @@
       <c r="A30" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="44">
+      <c r="B30" s="24">
         <v>45536</v>
       </c>
       <c r="C30" s="16"/>
@@ -2391,13 +2435,17 @@
       <c r="AQ30"/>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="18"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
+      <c r="A31" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="45">
+        <v>46001</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
       <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
       <c r="H31" s="16"/>
       <c r="I31"/>
       <c r="J31"/>
@@ -2436,14 +2484,18 @@
       <c r="AQ31"/>
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
-      <c r="B32" s="14"/>
+      <c r="A32" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="45">
+        <v>45947</v>
+      </c>
       <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
+      <c r="D32" s="17"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2481,13 +2533,15 @@
       <c r="AQ32"/>
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
+      <c r="A33" s="48" t="s">
+        <v>43</v>
+      </c>
       <c r="B33" s="14"/>
-      <c r="C33" s="16"/>
+      <c r="C33" s="17"/>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="G33" s="17"/>
       <c r="H33" s="16"/>
       <c r="I33"/>
       <c r="J33"/>
@@ -2663,6 +2717,11 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2670,11 +2729,6 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>